<commit_message>
Updated the framework with all the latest dependencies
</commit_message>
<xml_diff>
--- a/src/main/resources/config/VehicleData.xlsx
+++ b/src/main/resources/config/VehicleData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10610"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hemanths/Desktop/HMRC-Test/src/main/resources/config/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Viraj\LearningAndDevelopment\java-selenium-webdriver-bdd-demo\src\main\resources\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58AB472D-F555-0A48-9F36-DD84FDA5357A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE92B024-5AF1-48E7-8DD6-A195233A1E5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16480" tabRatio="990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="45780" yWindow="780" windowWidth="21600" windowHeight="11295" tabRatio="990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="VehicleData" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
   <si>
     <t>MAKE</t>
   </si>
@@ -94,6 +94,9 @@
   </si>
   <si>
     <t>VAUXHALL</t>
+  </si>
+  <si>
+    <t>JAGUAR</t>
   </si>
 </sst>
 </file>
@@ -142,7 +145,7 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -162,9 +165,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -202,7 +205,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -308,7 +311,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -450,7 +453,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -461,18 +464,18 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="1025" width="11.5"/>
+    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="1025" width="11.42578125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>15</v>
       </c>
@@ -483,7 +486,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>21</v>
       </c>
@@ -494,7 +497,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -505,7 +508,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -516,7 +519,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -527,7 +530,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>17</v>
       </c>
@@ -538,18 +541,18 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>2</v>
       </c>
@@ -560,7 +563,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>13</v>
       </c>

</xml_diff>